<commit_message>
cambiar nombre de campo a provincia, "provincia" por "Nombre"
</commit_message>
<xml_diff>
--- a/src/provincias.xlsx
+++ b/src/provincias.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedel\Documents\GitHub\demarcacion_administrativa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedel\Documents\GitHub\demarcacion_administrativa\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3463DDD9-449B-4A88-A759-8598E7376DE4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AABC51-521F-4826-A906-A42330DB9CC9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,6 @@
     <t>CPRO</t>
   </si>
   <si>
-    <t>Provincia</t>
-  </si>
-  <si>
     <t>CODAUTO</t>
   </si>
   <si>
@@ -341,6 +338,9 @@
   </si>
   <si>
     <t>Melilla</t>
+  </si>
+  <si>
+    <t>NOMBRE</t>
   </si>
 </sst>
 </file>
@@ -681,7 +681,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -690,582 +692,582 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>28</v>
-      </c>
-      <c r="C13" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
         <v>35</v>
       </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
         <v>37</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>38</v>
-      </c>
-      <c r="C17" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s">
         <v>41</v>
       </c>
-      <c r="B19" t="s">
-        <v>42</v>
-      </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
         <v>43</v>
       </c>
-      <c r="B20" t="s">
-        <v>44</v>
-      </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
         <v>45</v>
       </c>
-      <c r="B21" t="s">
-        <v>46</v>
-      </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
         <v>47</v>
       </c>
-      <c r="B22" t="s">
-        <v>48</v>
-      </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s">
         <v>49</v>
       </c>
-      <c r="B23" t="s">
-        <v>50</v>
-      </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
         <v>51</v>
       </c>
-      <c r="B24" t="s">
-        <v>52</v>
-      </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" t="s">
         <v>53</v>
       </c>
-      <c r="B25" t="s">
-        <v>54</v>
-      </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s">
         <v>55</v>
       </c>
-      <c r="B26" t="s">
-        <v>56</v>
-      </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" t="s">
         <v>57</v>
-      </c>
-      <c r="C27" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" t="s">
         <v>59</v>
       </c>
-      <c r="B28" t="s">
-        <v>60</v>
-      </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" t="s">
         <v>61</v>
       </c>
-      <c r="B29" t="s">
-        <v>62</v>
-      </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" t="s">
         <v>63</v>
       </c>
-      <c r="B30" t="s">
-        <v>64</v>
-      </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" t="s">
         <v>65</v>
       </c>
-      <c r="B31" t="s">
-        <v>66</v>
-      </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" t="s">
         <v>68</v>
       </c>
-      <c r="B33" t="s">
-        <v>69</v>
-      </c>
       <c r="C33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" t="s">
         <v>70</v>
       </c>
-      <c r="B34" t="s">
-        <v>71</v>
-      </c>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" t="s">
         <v>72</v>
       </c>
-      <c r="B35" t="s">
-        <v>73</v>
-      </c>
       <c r="C35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" t="s">
         <v>74</v>
-      </c>
-      <c r="C36" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" t="s">
         <v>76</v>
       </c>
-      <c r="B37" t="s">
-        <v>77</v>
-      </c>
       <c r="C37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" t="s">
         <v>78</v>
       </c>
-      <c r="B38" t="s">
-        <v>79</v>
-      </c>
       <c r="C38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" t="s">
         <v>82</v>
       </c>
-      <c r="B41" t="s">
-        <v>83</v>
-      </c>
       <c r="C41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" t="s">
         <v>84</v>
       </c>
-      <c r="B42" t="s">
-        <v>85</v>
-      </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" t="s">
         <v>86</v>
       </c>
-      <c r="B43" t="s">
-        <v>87</v>
-      </c>
       <c r="C43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" t="s">
         <v>88</v>
       </c>
-      <c r="B44" t="s">
-        <v>89</v>
-      </c>
       <c r="C44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" t="s">
         <v>90</v>
       </c>
-      <c r="B45" t="s">
-        <v>91</v>
-      </c>
       <c r="C45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" t="s">
         <v>92</v>
       </c>
-      <c r="B46" t="s">
-        <v>93</v>
-      </c>
       <c r="C46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" t="s">
         <v>94</v>
       </c>
-      <c r="B47" t="s">
-        <v>95</v>
-      </c>
       <c r="C47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" t="s">
         <v>97</v>
       </c>
-      <c r="B49" t="s">
-        <v>98</v>
-      </c>
       <c r="C49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" t="s">
         <v>99</v>
       </c>
-      <c r="B50" t="s">
-        <v>100</v>
-      </c>
       <c r="C50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" t="s">
         <v>101</v>
       </c>
-      <c r="B51" t="s">
-        <v>102</v>
-      </c>
       <c r="C51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" t="s">
         <v>103</v>
       </c>
-      <c r="B52" t="s">
-        <v>104</v>
-      </c>
       <c r="C52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" t="s">
         <v>105</v>
       </c>
-      <c r="B53" t="s">
-        <v>106</v>
-      </c>
       <c r="C53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>